<commit_message>
Fix: no pubDate wont fail anymore
</commit_message>
<xml_diff>
--- a/resources/explores.xlsx
+++ b/resources/explores.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10604\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86158\Desktop\GH-projects\JSS_Reader\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D5F00B-D6EA-45D8-81CC-09BEFD2B76DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745705AD-9E89-4B2B-BE8D-BFA778B0D6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{44B4CE17-E233-415A-B01D-403679C3053D}"/>
+    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{44B4CE17-E233-415A-B01D-403679C3053D}"/>
   </bookViews>
   <sheets>
     <sheet name="工作簿2" sheetId="1" r:id="rId1"/>
     <sheet name="备用" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作簿2!$A$1:$C$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作簿2!$A$1:$C$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,41 +29,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="87">
-  <si>
-    <t>https://rsshub.app/sjtu/seiee/academic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>电子信息与电气工程学院本科教务办</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
   <si>
     <t>电子信息与电气工程学院学生工作办公室</t>
   </si>
   <si>
-    <t>https://rsshub.app/sjtu/seiee/xsb/news</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>研究生通知公告</t>
   </si>
   <si>
-    <t>https://rsshub.app/sjtu/seiee/bjwb/major_select</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://rsshub.app/sjtu/gs/enroll/59</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sjtu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://rsshub.app/ctfhub/search</t>
-  </si>
-  <si>
-    <t>查询国内外 CTF 赛事信息</t>
   </si>
   <si>
     <t>https://rsshub.app/sjtu/jwc</t>
@@ -324,195 +298,212 @@
     <t>https://rsshub.app/bilibili/ranking/0/3/1</t>
   </si>
   <si>
+    <t>https://rsshub.app/pixiv/ranking/week</t>
+  </si>
+  <si>
+    <t>pixiv周排行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/douban/movie/playing</t>
+  </si>
+  <si>
+    <t>豆瓣：正在上映的电影</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/douban/movie/weekly</t>
+  </si>
+  <si>
+    <t>豆瓣：一周口碑榜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>豆瓣：新书速递</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/douban/book/latest</t>
+  </si>
+  <si>
+    <t>豆瓣：热门图书排行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/douban/book/rank/fiction</t>
+  </si>
+  <si>
+    <t>https://rsshub.app/zhihu/hotlist</t>
+  </si>
+  <si>
+    <t>https://rsshub.app/weibo/search/hot</t>
+  </si>
+  <si>
+    <t>微博热搜榜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/thepaper/featured</t>
+  </si>
+  <si>
+    <t>澎湃新闻：首页头条</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/ielts</t>
+  </si>
+  <si>
+    <t>雅思最新消息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/arknights/news</t>
+  </si>
+  <si>
+    <t>https://rsshub.app/tencent/pvp/newsindex/all</t>
+  </si>
+  <si>
+    <t>https://rsshub.app/lol/newsindex/all</t>
+  </si>
+  <si>
+    <t>steam史低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电子信息与电气工程学院学术动态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b站综合热门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b站排行榜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b站每周必看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>知乎热榜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>知乎日报</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/usenix/usenix-security-sympoium</t>
+  </si>
+  <si>
+    <t>https://rsshub.app/ieee-security/security-privacy</t>
+  </si>
+  <si>
+    <t>https://rsshub.app/ndss-symposium/ndss</t>
+  </si>
+  <si>
+    <t>IEEE Symposium on Security and Privacy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USENIX Security</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Network and Distributed System Security (NDSS) Symposium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>崩坏：星穹铁道最新资讯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原神最新资讯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>明日方舟游戏公告与新闻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王者荣耀新闻中心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英雄联盟国服新闻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>孙吧精品贴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询国内外 CTF 赛事信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/sjtu/gs/enroll/59</t>
+  </si>
+  <si>
+    <t>https://rsshub.app/mihoyo/ys/main/latest</t>
+  </si>
+  <si>
+    <t>https://rsshub.app/mihoyo/sr/zh-cn</t>
+  </si>
+  <si>
+    <t>https://rsshub.app/yxdzqb/low</t>
+  </si>
+  <si>
     <t>https://rsshub.app/bilibili/weekly</t>
-  </si>
-  <si>
-    <t>https://rsshub.app/pixiv/ranking/week</t>
-  </si>
-  <si>
-    <t>pixiv周排行</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://rsshub.app/douban/movie/playing</t>
-  </si>
-  <si>
-    <t>豆瓣：正在上映的电影</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://rsshub.app/douban/movie/weekly</t>
-  </si>
-  <si>
-    <t>豆瓣：一周口碑榜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>豆瓣：新书速递</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://rsshub.app/douban/book/latest</t>
-  </si>
-  <si>
-    <t>豆瓣：热门图书排行</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://rsshub.app/douban/book/rank/fiction</t>
-  </si>
-  <si>
-    <t>https://rsshub.app/zhihu/hotlist</t>
-  </si>
-  <si>
-    <t>https://rsshub.app/weibo/search/hot</t>
-  </si>
-  <si>
-    <t>微博热搜榜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://rsshub.app/thepaper/featured</t>
-  </si>
-  <si>
-    <t>澎湃新闻：首页头条</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://rsshub.app/ielts</t>
-  </si>
-  <si>
-    <t>雅思最新消息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rsshub.app/mihoyo/ys/main/latest</t>
-  </si>
-  <si>
-    <t>rsshub.app/mihoyo/sr/zh-cn</t>
-  </si>
-  <si>
-    <t>https://rsshub.app/arknights/news</t>
-  </si>
-  <si>
-    <t>https://rsshub.app/tencent/pvp/newsindex/all</t>
-  </si>
-  <si>
-    <t>https://rsshub.app/lol/newsindex/all</t>
-  </si>
-  <si>
-    <t>rsshub.app/yxdzqb/low</t>
-  </si>
-  <si>
-    <t>steam史低</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>娱乐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>资讯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>游戏</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>电子信息与电气工程学院学术动态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>水源社区最新帖子</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>水源社区最新话题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b站综合热门</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b站排行榜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b站每周必看</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>知乎热榜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>知乎日报</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://rsshub.app/usenix/usenix-security-sympoium</t>
-  </si>
-  <si>
-    <t>期刊</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://rsshub.app/ieee-security/security-privacy</t>
-  </si>
-  <si>
-    <t>https://rsshub.app/ndss-symposium/ndss</t>
-  </si>
-  <si>
-    <t>IEEE Symposium on Security and Privacy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USENIX Security</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Network and Distributed System Security (NDSS) Symposium</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rsshub.app/baidu/tieba/forum/good/孙笑川</t>
-  </si>
-  <si>
-    <t>资讯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>崩坏：星穹铁道最新资讯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>原神最新资讯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>明日方舟游戏公告与新闻</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>王者荣耀新闻中心</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>英雄联盟国服新闻</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>孙吧精品贴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://shuiyuan.sjtu.edu.cn/latest.rss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://shuiyuan.sjtu.edu.cn/posts.rss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gaming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SJTU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Journal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entertainment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/baidu/tieba/forum/good/孙笑川</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/nature/research/ng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nature (Nature Genetics) | Latest Research</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://feeds.science.org/rss/science.xml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Science</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/sjtu/seiee/xsb/news</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://rsshub.app/sjtu/seiee/academic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -931,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB08E850-C18E-4907-95C0-93B3B1955E81}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -946,412 +937,401 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="34.799999999999997" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>2</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C33" xr:uid="{DB08E850-C18E-4907-95C0-93B3B1955E81}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C33">
-      <sortCondition ref="C2:C33"/>
+  <autoFilter ref="A1:C31" xr:uid="{DB08E850-C18E-4907-95C0-93B3B1955E81}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C31">
+      <sortCondition ref="C2:C31"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C29">
-    <sortCondition ref="C2:C29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C27">
+    <sortCondition ref="C2:C27"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D252DDD4-DBD9-4F85-8121-8FE0B81590DC}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{AF475535-259A-4A06-943C-B5C984BA0FA0}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{FCB551AD-7039-4D73-B683-8DE8A8CEF6B8}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{16815FC6-DD7D-48E2-91AD-CCEB213C8ED8}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{E4ADAD8B-F58F-4889-9AC3-602F1ACD454A}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{48932E7B-0CC6-4BAC-8A66-D703EE3C9382}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{7227C1C1-7F4E-4CEA-9BCC-6CB57C303447}"/>
-    <hyperlink ref="A20" r:id="rId8" xr:uid="{5A9BDE65-6781-429A-A7C2-DDDD503BD2AE}"/>
-    <hyperlink ref="A21" r:id="rId9" xr:uid="{DDA7AE34-16E6-4C70-BD62-5878D526A752}"/>
-    <hyperlink ref="A22" r:id="rId10" xr:uid="{03C41D7E-FCF2-4ACC-BC91-AA79DA7A7306}"/>
-    <hyperlink ref="A23" r:id="rId11" xr:uid="{AD231F8B-B28C-4F84-B454-8E39F07F1753}"/>
-    <hyperlink ref="A24" r:id="rId12" xr:uid="{2730C138-D2E5-424E-8D09-7C27879CBBB7}"/>
-    <hyperlink ref="A25" r:id="rId13" xr:uid="{E1EBAF6B-0A4E-46F4-893B-8E66583BC8C3}"/>
-    <hyperlink ref="A26" r:id="rId14" xr:uid="{19469520-6A54-4F79-9E09-3A976611E624}"/>
-    <hyperlink ref="A27" r:id="rId15" xr:uid="{EE1F0039-9E92-4408-9FEE-3D83483EDB79}"/>
-    <hyperlink ref="A29" r:id="rId16" xr:uid="{DAE26C27-242E-437C-8CB9-9B33C8C824F8}"/>
-    <hyperlink ref="A28" r:id="rId17" xr:uid="{162DFAD1-9AFC-4044-AEF3-F7FA2D2D981D}"/>
-    <hyperlink ref="A30" r:id="rId18" xr:uid="{A21FA03A-302C-419B-A7D9-D8A2AFB9BBEB}"/>
-    <hyperlink ref="A31" r:id="rId19" xr:uid="{851E0977-E47A-4E03-8327-B8B91EA78088}"/>
-    <hyperlink ref="A32" r:id="rId20" xr:uid="{C52CA451-5E25-4EF7-95FD-1E9FF95E26FF}"/>
-    <hyperlink ref="A14" r:id="rId21" display="https://rsshub.app/mihoyo/ys/main/latest" xr:uid="{BDA91C5C-869B-4ED5-81F9-F10BECC758C7}"/>
-    <hyperlink ref="A15" r:id="rId22" display="https://rsshub.app/mihoyo/sr/zh-cn" xr:uid="{51EF2DBD-3075-48F4-A15C-6863F6A946BE}"/>
-    <hyperlink ref="A16" r:id="rId23" xr:uid="{32BC84DD-1ACD-4997-817E-806C5E622995}"/>
-    <hyperlink ref="A17" r:id="rId24" xr:uid="{760441AD-2778-4BA5-B10A-616FCA2F0875}"/>
-    <hyperlink ref="A18" r:id="rId25" xr:uid="{B8800C5D-042F-41E7-9C7E-E0DF97D2028C}"/>
-    <hyperlink ref="A19" r:id="rId26" display="https://rsshub.app/yxdzqb/low" xr:uid="{BC226CFC-5D86-4AE7-A318-C6B0A2E5BAB5}"/>
-    <hyperlink ref="A11" r:id="rId27" xr:uid="{34B7B70F-DD94-4EB7-968A-25488F2B4AF8}"/>
-    <hyperlink ref="A12" r:id="rId28" xr:uid="{499365FA-9872-4F55-A6D3-70B8A1723784}"/>
-    <hyperlink ref="A13" r:id="rId29" xr:uid="{EC7C6B04-3D96-4722-B427-9CF9BA180BDC}"/>
-    <hyperlink ref="A33" r:id="rId30" display="https://rsshub.app/baidu/tieba/forum/good/%E5%AD%99%E7%AC%91%E5%B7%9D" xr:uid="{FD82AB01-2946-4E06-A47E-640A0EFAD3FD}"/>
-    <hyperlink ref="A10" r:id="rId31" xr:uid="{63361BBD-912D-4530-9894-1F707E991CC7}"/>
-    <hyperlink ref="A9" r:id="rId32" xr:uid="{EF2E0835-60B5-48D9-8F4D-83CA077FACBC}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{FCB551AD-7039-4D73-B683-8DE8A8CEF6B8}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://rsshub.rssforever.com/sjtu/gs/enroll/59" xr:uid="{16815FC6-DD7D-48E2-91AD-CCEB213C8ED8}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{7227C1C1-7F4E-4CEA-9BCC-6CB57C303447}"/>
+    <hyperlink ref="A18" r:id="rId5" xr:uid="{5A9BDE65-6781-429A-A7C2-DDDD503BD2AE}"/>
+    <hyperlink ref="A19" r:id="rId6" xr:uid="{DDA7AE34-16E6-4C70-BD62-5878D526A752}"/>
+    <hyperlink ref="A20" r:id="rId7" xr:uid="{03C41D7E-FCF2-4ACC-BC91-AA79DA7A7306}"/>
+    <hyperlink ref="A21" r:id="rId8" xr:uid="{AD231F8B-B28C-4F84-B454-8E39F07F1753}"/>
+    <hyperlink ref="A22" r:id="rId9" xr:uid="{2730C138-D2E5-424E-8D09-7C27879CBBB7}"/>
+    <hyperlink ref="A23" r:id="rId10" xr:uid="{E1EBAF6B-0A4E-46F4-893B-8E66583BC8C3}"/>
+    <hyperlink ref="A24" r:id="rId11" xr:uid="{19469520-6A54-4F79-9E09-3A976611E624}"/>
+    <hyperlink ref="A25" r:id="rId12" xr:uid="{EE1F0039-9E92-4408-9FEE-3D83483EDB79}"/>
+    <hyperlink ref="A27" r:id="rId13" xr:uid="{DAE26C27-242E-437C-8CB9-9B33C8C824F8}"/>
+    <hyperlink ref="A26" r:id="rId14" xr:uid="{162DFAD1-9AFC-4044-AEF3-F7FA2D2D981D}"/>
+    <hyperlink ref="A28" r:id="rId15" xr:uid="{A21FA03A-302C-419B-A7D9-D8A2AFB9BBEB}"/>
+    <hyperlink ref="A29" r:id="rId16" xr:uid="{851E0977-E47A-4E03-8327-B8B91EA78088}"/>
+    <hyperlink ref="A30" r:id="rId17" xr:uid="{C52CA451-5E25-4EF7-95FD-1E9FF95E26FF}"/>
+    <hyperlink ref="A12" r:id="rId18" display="https://rsshub.rssforever.com/mihoyo/ys/main/latest" xr:uid="{BDA91C5C-869B-4ED5-81F9-F10BECC758C7}"/>
+    <hyperlink ref="A13" r:id="rId19" display="https://rsshub.rssforever.com/mihoyo/sr/zh-cn" xr:uid="{51EF2DBD-3075-48F4-A15C-6863F6A946BE}"/>
+    <hyperlink ref="A14" r:id="rId20" xr:uid="{32BC84DD-1ACD-4997-817E-806C5E622995}"/>
+    <hyperlink ref="A15" r:id="rId21" xr:uid="{760441AD-2778-4BA5-B10A-616FCA2F0875}"/>
+    <hyperlink ref="A16" r:id="rId22" xr:uid="{B8800C5D-042F-41E7-9C7E-E0DF97D2028C}"/>
+    <hyperlink ref="A17" r:id="rId23" display="https://rsshub.rssforever.com/yxdzqb/low" xr:uid="{BC226CFC-5D86-4AE7-A318-C6B0A2E5BAB5}"/>
+    <hyperlink ref="A7" r:id="rId24" display="https://rsshub.rssforever.com/usenix/usenix-security-sympoium" xr:uid="{34B7B70F-DD94-4EB7-968A-25488F2B4AF8}"/>
+    <hyperlink ref="A8" r:id="rId25" xr:uid="{499365FA-9872-4F55-A6D3-70B8A1723784}"/>
+    <hyperlink ref="A9" r:id="rId26" xr:uid="{EC7C6B04-3D96-4722-B427-9CF9BA180BDC}"/>
+    <hyperlink ref="A31" r:id="rId27" xr:uid="{FD82AB01-2946-4E06-A47E-640A0EFAD3FD}"/>
+    <hyperlink ref="A32" r:id="rId28" display="https://rsshub.rssforever.com/ctfhub/search" xr:uid="{82F1B067-24A0-4E03-89D6-2716327A63AC}"/>
+    <hyperlink ref="A10" r:id="rId29" xr:uid="{4DD09D7D-5334-4CFA-B96F-174B353A1922}"/>
+    <hyperlink ref="A11" r:id="rId30" xr:uid="{786DF078-221E-47BB-ABE2-9A840FCCEDF5}"/>
+    <hyperlink ref="A5" r:id="rId31" xr:uid="{48932E7B-0CC6-4BAC-8A66-D703EE3C9382}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
@@ -1371,58 +1351,58 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>